<commit_message>
Enhance trajectory charts with dynamic titles; update default selection in histogram UI; modify bundle ID in deployment configuration; update DFC template.
</commit_message>
<xml_diff>
--- a/templates/Template-DFC.xlsx
+++ b/templates/Template-DFC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://incorporadoraampla.sharepoint.com/sites/Controladoria/Documentos Compartilhados/amplaGitHub/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{482EB0F2-8EC4-40C5-8B55-F33B1732A6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{487FF841-5A3B-41CA-9BAB-7F8EA65C3518}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="8_{482EB0F2-8EC4-40C5-8B55-F33B1732A6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC8A2A15-0FE4-4FE5-9B8C-3CBEB2F74AF7}"/>
   <bookViews>
     <workbookView xWindow="-57600" yWindow="-3555" windowWidth="14400" windowHeight="7800" xr2:uid="{E8652140-B299-493A-AAA8-27682F0F7EF9}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Por empresa" sheetId="1" r:id="rId1"/>
     <sheet name="Por empreendimento" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Código</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Pró soluto</t>
   </si>
   <si>
-    <t>Entradas operacionais</t>
-  </si>
-  <si>
     <t>Pagamentos a fornecedores</t>
   </si>
   <si>
@@ -121,13 +118,67 @@
   </si>
   <si>
     <t>Caixa líquido das atividades operacionais</t>
+  </si>
+  <si>
+    <t>Venda de ativos imobilizados / terrenos</t>
+  </si>
+  <si>
+    <t>Recebimento de juros sobre aplicações</t>
+  </si>
+  <si>
+    <t>Aquisição de terrenos</t>
+  </si>
+  <si>
+    <t>Investimento em construção e obras em andamento</t>
+  </si>
+  <si>
+    <t>Aquisição de equipamentos</t>
+  </si>
+  <si>
+    <t>Investimento em participações / SPEs</t>
+  </si>
+  <si>
+    <t>Entradas de atividades de investimento</t>
+  </si>
+  <si>
+    <t>Captação de empréstimos / financiamentos bancários</t>
+  </si>
+  <si>
+    <t>Aporte de capital dos sócios</t>
+  </si>
+  <si>
+    <t>Entradas de atividades operacionais</t>
+  </si>
+  <si>
+    <t>Saídas de atividades operacionais</t>
+  </si>
+  <si>
+    <t>Saídas de atividades de investimento</t>
+  </si>
+  <si>
+    <t>Caixa líquido das atividades de investimento</t>
+  </si>
+  <si>
+    <t>Entradas de atividades de financiamento</t>
+  </si>
+  <si>
+    <t>Amortização de empréstimos / financiamentos</t>
+  </si>
+  <si>
+    <t>Pagamento de juros</t>
+  </si>
+  <si>
+    <t>Distribuição de dividendos / JCP</t>
+  </si>
+  <si>
+    <t>Saídas de atividades de financiamento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,13 +186,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -156,9 +245,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,126 +609,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93FF019-ACA5-4674-AAA1-FFC1EFB894DF}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="53.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="1" t="s">
+    </row>
+    <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B24" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B32" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -633,4 +855,231 @@
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006C56FB2846673243A9735D5EC6051572" ma:contentTypeVersion="11" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="36569ac63cfce8ff0f8884bc80e67f1c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5a5f483f-f768-438e-b4ef-63f46a7558dd" xmlns:ns3="dd8c73df-45bd-468c-aae5-f3faedcbd5e2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2040da04b75a9ea4fe796fa8180f8ca6" ns2:_="" ns3:_="">
+    <xsd:import namespace="5a5f483f-f768-438e-b4ef-63f46a7558dd"/>
+    <xsd:import namespace="dd8c73df-45bd-468c-aae5-f3faedcbd5e2"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5a5f483f-f768-438e-b4ef-63f46a7558dd" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Marcações de imagem" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="d52aaf24-8448-430e-97e8-d28c57d898a4" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="dd8c73df-45bd-468c-aae5-f3faedcbd5e2" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{6bacedc3-d3dc-49dd-a723-47ba9b97a11c}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="dd8c73df-45bd-468c-aae5-f3faedcbd5e2">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de Conteúdo"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5a5f483f-f768-438e-b4ef-63f46a7558dd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="dd8c73df-45bd-468c-aae5-f3faedcbd5e2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6EC9A054-2C10-46A1-9B76-ACBA99CCF3CA}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D0C9ED-A4CF-4CCD-9195-4E5E5B64A93C}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60C6D15D-69FE-4513-A04A-B82A30A7A069}"/>
 </file>
</xml_diff>

<commit_message>
Refactor Despesas trajectory chart server module for improved data handling; add dynamic chart title and click event observer; update bundle ID in deployment configuration; modify DFC template.
</commit_message>
<xml_diff>
--- a/templates/Template-DFC.xlsx
+++ b/templates/Template-DFC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://incorporadoraampla.sharepoint.com/sites/Controladoria/Documentos Compartilhados/amplaGitHub/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{482EB0F2-8EC4-40C5-8B55-F33B1732A6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC8A2A15-0FE4-4FE5-9B8C-3CBEB2F74AF7}"/>
+  <xr:revisionPtr revIDLastSave="166" documentId="8_{482EB0F2-8EC4-40C5-8B55-F33B1732A6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DE2372A-3B9E-4CFC-B995-A70F6B41A4A7}"/>
   <bookViews>
-    <workbookView xWindow="-57600" yWindow="-3555" windowWidth="14400" windowHeight="7800" xr2:uid="{E8652140-B299-493A-AAA8-27682F0F7EF9}"/>
+    <workbookView xWindow="-57600" yWindow="-3555" windowWidth="14400" windowHeight="15600" xr2:uid="{E8652140-B299-493A-AAA8-27682F0F7EF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Por empresa" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="46">
   <si>
     <t>Código</t>
   </si>
@@ -57,27 +57,12 @@
     <t>3.</t>
   </si>
   <si>
-    <t>4.</t>
-  </si>
-  <si>
     <t>Atividades de investimento</t>
   </si>
   <si>
     <t>Atividades de financiamento</t>
   </si>
   <si>
-    <t>Variação e saldos de caixa</t>
-  </si>
-  <si>
-    <t>1.1.</t>
-  </si>
-  <si>
-    <t>1.2.</t>
-  </si>
-  <si>
-    <t>1.3.</t>
-  </si>
-  <si>
     <t>Repasse</t>
   </si>
   <si>
@@ -87,33 +72,18 @@
     <t>Pagamentos a fornecedores</t>
   </si>
   <si>
-    <t>1.4.</t>
-  </si>
-  <si>
     <t>Pagamentos a empreiteiros/subempreiteiros</t>
   </si>
   <si>
-    <t>1.5.</t>
-  </si>
-  <si>
-    <t>1.6.</t>
-  </si>
-  <si>
     <t>Pagamentos de salários e encargos</t>
   </si>
   <si>
     <t>Despesas comerciais e de marketing</t>
   </si>
   <si>
-    <t>1.7.</t>
-  </si>
-  <si>
     <t>Despesas administrativas gerais</t>
   </si>
   <si>
-    <t>1.8.</t>
-  </si>
-  <si>
     <t>Impostos e contribuições sobre a receita</t>
   </si>
   <si>
@@ -172,13 +142,46 @@
   </si>
   <si>
     <t>Saídas de atividades de financiamento</t>
+  </si>
+  <si>
+    <t>Caixa líquido das atividades de financiamento</t>
+  </si>
+  <si>
+    <t>Variação líquida de caixa no período</t>
+  </si>
+  <si>
+    <t>Caixa e equivalentes no início do período</t>
+  </si>
+  <si>
+    <t>Caixa e equivalentes no fim do período</t>
+  </si>
+  <si>
+    <t>Origem</t>
+  </si>
+  <si>
+    <t>Arquivo</t>
+  </si>
+  <si>
+    <t>Tabela</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Observações</t>
+  </si>
+  <si>
+    <t>CEF</t>
+  </si>
+  <si>
+    <t>Informakon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +191,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Aptos Narrow"/>
@@ -245,9 +255,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -274,6 +285,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -609,234 +650,466 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93FF019-ACA5-4674-AAA1-FFC1EFB894DF}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="53.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="C2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6" t="s">
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+    </row>
+    <row r="17" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="19"/>
+    </row>
+    <row r="18" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="20"/>
+    </row>
+    <row r="23" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="17"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="13"/>
+    </row>
+    <row r="25" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="19"/>
+    </row>
+    <row r="28" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+    </row>
+    <row r="29" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+    </row>
+    <row r="30" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+    </row>
+    <row r="31" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="20"/>
+    </row>
+    <row r="32" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" s="17"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7" t="s">
+      <c r="C33" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" s="21"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9" t="s">
+      <c r="C34" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="21"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C35" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1073,13 +1346,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6EC9A054-2C10-46A1-9B76-ACBA99CCF3CA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5F1B5B1-5FBC-42BF-93E0-A1561CA25062}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D0C9ED-A4CF-4CCD-9195-4E5E5B64A93C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7BFC80B-7A55-4801-9844-CCCBA392669F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60C6D15D-69FE-4513-A04A-B82A30A7A069}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7E4AD77-7BCF-4163-8EFB-17D24A162300}"/>
 </file>
</xml_diff>

<commit_message>
Refactor m_edges, m_nodes, and m_gnw functions for improved edge and node definitions; update color handling in m_edges; modify deployment configuration with new bundle ID; add new dataset for enhanced functionality; update Template-DFC.xlsx.
</commit_message>
<xml_diff>
--- a/templates/Template-DFC.xlsx
+++ b/templates/Template-DFC.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://incorporadoraampla.sharepoint.com/sites/Controladoria/Documentos Compartilhados/amplaGitHub/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="8_{482EB0F2-8EC4-40C5-8B55-F33B1732A6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DE2372A-3B9E-4CFC-B995-A70F6B41A4A7}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="8_{482EB0F2-8EC4-40C5-8B55-F33B1732A6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D7C85B9-1EA7-46D5-9F68-FB54641EBF24}"/>
   <bookViews>
-    <workbookView xWindow="-57600" yWindow="-3555" windowWidth="14400" windowHeight="15600" xr2:uid="{E8652140-B299-493A-AAA8-27682F0F7EF9}"/>
+    <workbookView xWindow="-28920" yWindow="-1305" windowWidth="29040" windowHeight="15840" xr2:uid="{E8652140-B299-493A-AAA8-27682F0F7EF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Por empresa" sheetId="1" r:id="rId1"/>
     <sheet name="Por empreendimento" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -255,9 +255,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -265,43 +264,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -311,6 +289,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -653,7 +634,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -664,452 +645,452 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="13"/>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5" t="s">
+      <c r="C2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7" t="s">
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="15"/>
-    </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5" t="s">
+      <c r="C5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-    </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-    </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="16"/>
-    </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9" t="s">
+      <c r="C12" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="1:6" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6" t="s">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-    </row>
-    <row r="16" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6" t="s">
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-    </row>
-    <row r="17" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11" t="s">
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="19"/>
-    </row>
-    <row r="18" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6" t="s">
+      <c r="C17" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-    </row>
-    <row r="19" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6" t="s">
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-    </row>
-    <row r="20" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6" t="s">
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-    </row>
-    <row r="21" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6" t="s">
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-    </row>
-    <row r="22" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10" t="s">
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="20"/>
-    </row>
-    <row r="23" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9" t="s">
+      <c r="C22" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="17"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="C23" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="13"/>
+    </row>
+    <row r="24" spans="1:6" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" s="13"/>
-    </row>
-    <row r="25" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6" t="s">
+      <c r="C24" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-    </row>
-    <row r="26" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6" t="s">
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-    </row>
-    <row r="27" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11" t="s">
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+    </row>
+    <row r="27" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="F27" s="19"/>
-    </row>
-    <row r="28" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6" t="s">
+      <c r="C27" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-    </row>
-    <row r="29" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6" t="s">
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+    </row>
+    <row r="29" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-    </row>
-    <row r="30" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6" t="s">
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+    </row>
+    <row r="30" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-    </row>
-    <row r="31" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10" t="s">
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+    </row>
+    <row r="31" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="E31" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" s="20"/>
-    </row>
-    <row r="32" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9" t="s">
+      <c r="C31" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="12"/>
+    </row>
+    <row r="32" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F32" s="17"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12" t="s">
+      <c r="C32" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" s="13"/>
+    </row>
+    <row r="33" spans="1:6" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D33" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F33" s="21"/>
+      <c r="C33" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2" t="s">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F34" s="21"/>
+      <c r="C34" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2" t="s">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D35" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E35" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F35" s="21"/>
+      <c r="C35" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1326,15 +1307,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="5a5f483f-f768-438e-b4ef-63f46a7558dd">
@@ -1345,14 +1317,49 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5F1B5B1-5FBC-42BF-93E0-A1561CA25062}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5F1B5B1-5FBC-42BF-93E0-A1561CA25062}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5a5f483f-f768-438e-b4ef-63f46a7558dd"/>
+    <ds:schemaRef ds:uri="dd8c73df-45bd-468c-aae5-f3faedcbd5e2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7BFC80B-7A55-4801-9844-CCCBA392669F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7E4AD77-7BCF-4163-8EFB-17D24A162300}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5a5f483f-f768-438e-b4ef-63f46a7558dd"/>
+    <ds:schemaRef ds:uri="dd8c73df-45bd-468c-aae5-f3faedcbd5e2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7E4AD77-7BCF-4163-8EFB-17D24A162300}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7BFC80B-7A55-4801-9844-CCCBA392669F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Enhance g_desp.traj module by implementing multi-select functionality for improved data filtering; update app layout to include Select2 library for better UI experience. Modify deployment configuration with new bundle ID.
</commit_message>
<xml_diff>
--- a/templates/Template-DFC.xlsx
+++ b/templates/Template-DFC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://incorporadoraampla.sharepoint.com/sites/Controladoria/Documentos Compartilhados/amplaGitHub/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="167" documentId="8_{482EB0F2-8EC4-40C5-8B55-F33B1732A6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D7C85B9-1EA7-46D5-9F68-FB54641EBF24}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="8_{482EB0F2-8EC4-40C5-8B55-F33B1732A6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B1C05BF-C9AD-4705-A08C-0679DA1D7A42}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1305" windowWidth="29040" windowHeight="15840" xr2:uid="{E8652140-B299-493A-AAA8-27682F0F7EF9}"/>
+    <workbookView xWindow="-57600" yWindow="-3555" windowWidth="14400" windowHeight="15600" xr2:uid="{E8652140-B299-493A-AAA8-27682F0F7EF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Por empresa" sheetId="1" r:id="rId1"/>
@@ -634,7 +634,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -682,7 +682,7 @@
       </c>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -694,7 +694,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
         <v>9</v>
@@ -706,7 +706,7 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5" t="s">
         <v>26</v>
@@ -722,7 +722,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
@@ -732,7 +732,7 @@
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
@@ -742,7 +742,7 @@
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
@@ -752,7 +752,7 @@
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
@@ -762,7 +762,7 @@
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
     </row>
-    <row r="10" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
@@ -772,7 +772,7 @@
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
@@ -782,7 +782,7 @@
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>27</v>
@@ -798,7 +798,7 @@
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7" t="s">
         <v>16</v>
@@ -808,7 +808,7 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
     </row>
-    <row r="14" spans="1:6" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
@@ -820,7 +820,7 @@
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
         <v>17</v>
@@ -830,7 +830,7 @@
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
         <v>18</v>
@@ -840,7 +840,7 @@
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
     </row>
-    <row r="17" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
         <v>23</v>
@@ -856,7 +856,7 @@
       </c>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
         <v>19</v>
@@ -866,7 +866,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
     </row>
-    <row r="19" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
         <v>20</v>
@@ -876,7 +876,7 @@
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
     </row>
-    <row r="20" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
         <v>21</v>
@@ -886,7 +886,7 @@
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
         <v>22</v>
@@ -896,7 +896,7 @@
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
     </row>
-    <row r="22" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6" t="s">
         <v>28</v>
@@ -912,7 +912,7 @@
       </c>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7" t="s">
         <v>29</v>
@@ -928,7 +928,7 @@
       </c>
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="1:6" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
@@ -946,7 +946,7 @@
       </c>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
         <v>24</v>
@@ -956,7 +956,7 @@
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
         <v>25</v>
@@ -966,7 +966,7 @@
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="s">
         <v>30</v>
@@ -982,7 +982,7 @@
       </c>
       <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
         <v>31</v>
@@ -992,7 +992,7 @@
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
     </row>
-    <row r="29" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
         <v>32</v>
@@ -1002,7 +1002,7 @@
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
     </row>
-    <row r="30" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4" t="s">
         <v>33</v>
@@ -1012,7 +1012,7 @@
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
     </row>
-    <row r="31" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6" t="s">
         <v>34</v>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="F31" s="12"/>
     </row>
-    <row r="32" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7" t="s">
         <v>35</v>
@@ -1044,7 +1044,7 @@
       </c>
       <c r="F32" s="13"/>
     </row>
-    <row r="33" spans="1:6" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="8" t="s">
         <v>36</v>
@@ -1307,6 +1307,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="5a5f483f-f768-438e-b4ef-63f46a7558dd">
@@ -1315,15 +1324,6 @@
     <TaxCatchAll xmlns="dd8c73df-45bd-468c-aae5-f3faedcbd5e2" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1346,6 +1346,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7BFC80B-7A55-4801-9844-CCCBA392669F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7E4AD77-7BCF-4163-8EFB-17D24A162300}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1354,12 +1362,4 @@
     <ds:schemaRef ds:uri="dd8c73df-45bd-468c-aae5-f3faedcbd5e2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7BFC80B-7A55-4801-9844-CCCBA392669F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update Template-DFC.xlsx with new data structure and formatting improvements.
</commit_message>
<xml_diff>
--- a/templates/Template-DFC.xlsx
+++ b/templates/Template-DFC.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://incorporadoraampla.sharepoint.com/sites/Controladoria/Documentos Compartilhados/amplaGitHub/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="8_{482EB0F2-8EC4-40C5-8B55-F33B1732A6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B1C05BF-C9AD-4705-A08C-0679DA1D7A42}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="8_{482EB0F2-8EC4-40C5-8B55-F33B1732A6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0930E05C-36C3-4413-8E55-2A148E38CDFA}"/>
   <bookViews>
-    <workbookView xWindow="-57600" yWindow="-3555" windowWidth="14400" windowHeight="15600" xr2:uid="{E8652140-B299-493A-AAA8-27682F0F7EF9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E8652140-B299-493A-AAA8-27682F0F7EF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Por empresa" sheetId="1" r:id="rId1"/>
     <sheet name="Por empreendimento" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
   <si>
     <t>Código</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>Informakon</t>
+  </si>
+  <si>
+    <t>extcef</t>
+  </si>
+  <si>
+    <t>rec</t>
   </si>
 </sst>
 </file>
@@ -634,7 +640,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -690,7 +696,9 @@
       <c r="C3" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
     </row>
@@ -702,7 +710,9 @@
       <c r="C4" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
@@ -951,8 +961,12 @@
       <c r="B25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
+      <c r="C25" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
     </row>

</xml_diff>

<commit_message>
Add gs_barras.empilhadas.mes module; implement UI and server logic for stacked bar and line plots, including reactive data handling and date filtering. Update bundle ID in deployment configuration.
</commit_message>
<xml_diff>
--- a/templates/Template-DFC.xlsx
+++ b/templates/Template-DFC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://incorporadoraampla.sharepoint.com/sites/Controladoria/Documentos Compartilhados/amplaGitHub/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="172" documentId="8_{482EB0F2-8EC4-40C5-8B55-F33B1732A6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0930E05C-36C3-4413-8E55-2A148E38CDFA}"/>
+  <xr:revisionPtr revIDLastSave="190" documentId="8_{482EB0F2-8EC4-40C5-8B55-F33B1732A6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDE83E90-7466-487A-A29D-3DC153A12258}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E8652140-B299-493A-AAA8-27682F0F7EF9}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Por empresa" sheetId="1" r:id="rId1"/>
     <sheet name="Por empreendimento" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
   <si>
     <t>Código</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Atividades de financiamento</t>
   </si>
   <si>
-    <t>Repasse</t>
-  </si>
-  <si>
     <t>Pró soluto</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>Despesas administrativas gerais</t>
   </si>
   <si>
-    <t>Impostos e contribuições sobre a receita</t>
-  </si>
-  <si>
     <t>Caixa líquido das atividades operacionais</t>
   </si>
   <si>
@@ -181,6 +175,12 @@
   </si>
   <si>
     <t>rec</t>
+  </si>
+  <si>
+    <t>Repasse PF da CEF</t>
+  </si>
+  <si>
+    <t>Impostos e outras despesas legais</t>
   </si>
 </sst>
 </file>
@@ -640,10 +640,10 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="53.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -658,16 +658,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -678,114 +678,118 @@
         <v>3</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
     </row>
-    <row r="10" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -795,23 +799,23 @@
     <row r="12" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
@@ -830,20 +834,20 @@
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
@@ -853,53 +857,53 @@
     <row r="17" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
     </row>
-    <row r="19" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
     </row>
-    <row r="20" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -909,32 +913,32 @@
     <row r="22" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F23" s="13"/>
     </row>
@@ -946,34 +950,36 @@
         <v>7</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C25" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="10"/>
+      <c r="E25" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="F25" s="10"/>
     </row>
-    <row r="26" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -983,43 +989,43 @@
     <row r="27" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
     </row>
-    <row r="29" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
     </row>
-    <row r="30" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
@@ -1029,80 +1035,80 @@
     <row r="31" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F31" s="12"/>
     </row>
     <row r="32" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F32" s="13"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F35" s="14"/>
     </row>

</xml_diff>

<commit_message>
Refactor CEF functions: rename e_cef_extrato to e_cef_extcef and e_cef_extratos to e_cef_extcefs; update references in documentation and code. Update bundle ID in deployment configuration.
</commit_message>
<xml_diff>
--- a/templates/Template-DFC.xlsx
+++ b/templates/Template-DFC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://incorporadoraampla.sharepoint.com/sites/Controladoria/Documentos Compartilhados/amplaGitHub/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="190" documentId="8_{482EB0F2-8EC4-40C5-8B55-F33B1732A6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDE83E90-7466-487A-A29D-3DC153A12258}"/>
+  <xr:revisionPtr revIDLastSave="198" documentId="8_{482EB0F2-8EC4-40C5-8B55-F33B1732A6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55FC653C-C221-486A-A344-A744A9E94705}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E8652140-B299-493A-AAA8-27682F0F7EF9}"/>
+    <workbookView xWindow="-14400" yWindow="-1185" windowWidth="14400" windowHeight="15600" xr2:uid="{E8652140-B299-493A-AAA8-27682F0F7EF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Por empresa" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
   <si>
     <t>Código</t>
   </si>
@@ -168,13 +168,7 @@
     <t>CEF</t>
   </si>
   <si>
-    <t>Informakon</t>
-  </si>
-  <si>
     <t>extcef</t>
-  </si>
-  <si>
-    <t>rec</t>
   </si>
   <si>
     <t>Repasse PF da CEF</t>
@@ -640,7 +634,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -691,16 +685,16 @@
     <row r="3" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>42</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3" s="10"/>
     </row>
@@ -709,15 +703,9 @@
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>45</v>
-      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -789,7 +777,7 @@
     <row r="11" spans="1:6" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -969,10 +957,10 @@
         <v>42</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F25" s="10"/>
     </row>

</xml_diff>